<commit_message>
addded a text document
</commit_message>
<xml_diff>
--- a/WBS_Buck.xlsx
+++ b/WBS_Buck.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Buck\Desktop\PCSim\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA7C566-7268-4057-94EE-E45D63854BE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12195" yWindow="465" windowWidth="16920" windowHeight="12900" tabRatio="500"/>
+    <workbookView xWindow="12195" yWindow="465" windowWidth="16920" windowHeight="12900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS Diagram" sheetId="1" r:id="rId1"/>
@@ -127,7 +133,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -342,7 +348,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -382,6 +388,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -400,8 +409,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -412,16 +427,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -433,9 +439,10 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -482,7 +489,7 @@
         <xdr:cNvPr id="42" name="Straight Connector 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -537,7 +544,7 @@
         <xdr:cNvPr id="56" name="Straight Connector 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000038000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -592,7 +599,7 @@
         <xdr:cNvPr id="43" name="Straight Connector 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -647,7 +654,7 @@
         <xdr:cNvPr id="44" name="Straight Connector 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -702,7 +709,7 @@
         <xdr:cNvPr id="45" name="Straight Connector 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -757,7 +764,7 @@
         <xdr:cNvPr id="46" name="Straight Connector 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -812,7 +819,7 @@
         <xdr:cNvPr id="47" name="Straight Connector 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -867,7 +874,7 @@
         <xdr:cNvPr id="48" name="Straight Connector 47">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000030000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -922,7 +929,7 @@
         <xdr:cNvPr id="49" name="Straight Connector 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000031000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -977,7 +984,7 @@
         <xdr:cNvPr id="50" name="Straight Connector 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000032000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1032,7 +1039,7 @@
         <xdr:cNvPr id="55" name="Straight Connector 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000037000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1087,7 +1094,7 @@
         <xdr:cNvPr id="60" name="Straight Connector 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1142,7 +1149,7 @@
         <xdr:cNvPr id="61" name="Straight Connector 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1197,7 +1204,7 @@
         <xdr:cNvPr id="62" name="Straight Connector 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1252,7 +1259,7 @@
         <xdr:cNvPr id="63" name="Straight Connector 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1307,7 +1314,7 @@
         <xdr:cNvPr id="64" name="Straight Connector 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000040000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000040000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1362,7 +1369,7 @@
         <xdr:cNvPr id="65" name="Straight Connector 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000041000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000041000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1417,7 +1424,7 @@
         <xdr:cNvPr id="66" name="Straight Connector 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000042000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1472,7 +1479,7 @@
         <xdr:cNvPr id="67" name="Straight Connector 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000043000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1527,7 +1534,7 @@
         <xdr:cNvPr id="68" name="Straight Connector 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000044000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1582,7 +1589,7 @@
         <xdr:cNvPr id="70" name="Straight Connector 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000046000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000046000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1637,7 +1644,7 @@
         <xdr:cNvPr id="71" name="Straight Connector 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000047000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1692,7 +1699,7 @@
         <xdr:cNvPr id="72" name="Straight Connector 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000048000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000048000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1747,7 +1754,7 @@
         <xdr:cNvPr id="73" name="Straight Connector 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000049000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1802,7 +1809,7 @@
         <xdr:cNvPr id="74" name="Straight Connector 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1857,7 +1864,7 @@
         <xdr:cNvPr id="75" name="Straight Connector 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1912,7 +1919,7 @@
         <xdr:cNvPr id="76" name="Straight Connector 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1967,7 +1974,7 @@
         <xdr:cNvPr id="77" name="Straight Connector 76">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2022,7 +2029,7 @@
         <xdr:cNvPr id="78" name="Straight Connector 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00004E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2031,501 +2038,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8145116" y="2914725"/>
-          <a:ext cx="2185416" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>346075</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>346075</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="80" name="Straight Connector 79">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000050000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12919075" y="2108200"/>
-          <a:ext cx="0" cy="381000"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1308100</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>68820</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1308100</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>223529</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="81" name="Straight Connector 80">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000051000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11829523" y="2920045"/>
-          <a:ext cx="0" cy="385618"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>346075</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>68820</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>346075</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>223529</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="82" name="Straight Connector 81">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000052000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12925601" y="2920045"/>
-          <a:ext cx="0" cy="385618"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1422400</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>68820</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1422400</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>223529</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="83" name="Straight Connector 82">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000053000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14001926" y="2920045"/>
-          <a:ext cx="0" cy="385618"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>346075</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>346075</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="84" name="Straight Connector 83">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000054000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12919075" y="2540000"/>
-          <a:ext cx="0" cy="381000"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>346075</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>346075</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="85" name="Straight Connector 84">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000055000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12919075" y="3467100"/>
-          <a:ext cx="0" cy="685800"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1425575</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1425575</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="86" name="Straight Connector 85">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000056000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13998575" y="3467100"/>
-          <a:ext cx="0" cy="685800"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1311275</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1311275</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="87" name="Straight Connector 86">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000057000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11826875" y="3467100"/>
-          <a:ext cx="0" cy="685800"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1300419</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1427732</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="88" name="Straight Connector 87">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000058000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11821842" y="2914725"/>
           <a:ext cx="2185416" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2573,7 +2085,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2617,10 +2129,10 @@
         <xdr:cNvPr id="4" name="TextBox 3" title="Beeba's Law">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2701,7 +2213,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2795,7 +2307,7 @@
         <xdr:cNvPr id="9" name="TextBox 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2876,7 +2388,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2957,7 +2469,7 @@
         <xdr:cNvPr id="11" name="TextBox 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3038,7 +2550,7 @@
         <xdr:cNvPr id="13" name="TextBox 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3218,7 +2730,7 @@
         <xdr:cNvPr id="14" name="TextBox 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3364,7 +2876,7 @@
         <xdr:cNvPr id="15" name="TextBox 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3515,7 +3027,7 @@
         <xdr:cNvPr id="18" name="TextBox 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3579,7 +3091,7 @@
               <a:ea typeface="Century Gothic" charset="0"/>
               <a:cs typeface="Century Gothic" charset="0"/>
             </a:rPr>
-            <a:t> Designing/Office 1</a:t>
+            <a:t> Designi\/Office 1</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1000">
             <a:latin typeface="Century Gothic" charset="0"/>
@@ -3609,7 +3121,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3711,7 +3223,7 @@
         <xdr:cNvPr id="20" name="TextBox 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3805,7 +3317,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3907,7 +3419,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4047,7 +3559,7 @@
         <xdr:cNvPr id="23" name="TextBox 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4187,7 +3699,7 @@
         <xdr:cNvPr id="24" name="TextBox 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4298,7 +3810,7 @@
         <xdr:cNvPr id="26" name="TextBox 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4379,7 +3891,7 @@
         <xdr:cNvPr id="27" name="TextBox 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4473,7 +3985,7 @@
         <xdr:cNvPr id="28" name="TextBox 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4567,7 +4079,7 @@
         <xdr:cNvPr id="29" name="TextBox 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4664,7 +4176,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4800,7 +4312,7 @@
         <xdr:cNvPr id="31" name="TextBox 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4951,7 +4463,7 @@
         <xdr:cNvPr id="32" name="TextBox 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5031,14 +4543,6 @@
         </a:p>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="900" baseline="0">
               <a:latin typeface="Century Gothic" charset="0"/>
@@ -5053,763 +4557,6 @@
               <a:cs typeface="Century Gothic" charset="0"/>
             </a:rPr>
             <a:t>3.3.3 Print fllyers and anything else related.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>977900</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1663700</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="TextBox 33">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000022000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11493500" y="2286000"/>
-          <a:ext cx="2743200" cy="457200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="12700" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="12700" dir="5400000" algn="t" rotWithShape="0">
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="40000"/>
-            </a:schemeClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>Phase</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t> 4: Delivery/Closing</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1000">
-            <a:latin typeface="Century Gothic" charset="0"/>
-            <a:ea typeface="Century Gothic" charset="0"/>
-            <a:cs typeface="Century Gothic" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1727200</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="TextBox 34">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11328400" y="3086100"/>
-          <a:ext cx="914400" cy="546100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="12700" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="12700" dir="5400000" algn="t" rotWithShape="0">
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="40000"/>
-            </a:schemeClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>4.1 Social</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t> Media Campaigns</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="900">
-            <a:latin typeface="Century Gothic" charset="0"/>
-            <a:ea typeface="Century Gothic" charset="0"/>
-            <a:cs typeface="Century Gothic" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1898650</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>802821</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>217714</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="TextBox 35">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12403364" y="3100614"/>
-          <a:ext cx="958850" cy="654957"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="12700" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="12700" dir="5400000" algn="t" rotWithShape="0">
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="40000"/>
-            </a:schemeClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>4.2 Marketing Campaigns</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>927099</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>25401</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>2041070</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>54430</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="37" name="TextBox 36">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000025000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13486492" y="3100615"/>
-          <a:ext cx="1113971" cy="491672"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="12700" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="12700" dir="5400000" algn="t" rotWithShape="0">
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="40000"/>
-            </a:schemeClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>4.3 put</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t> up and hand out</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="900">
-            <a:latin typeface="Century Gothic" charset="0"/>
-            <a:ea typeface="Century Gothic" charset="0"/>
-            <a:cs typeface="Century Gothic" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>503466</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1905000</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>136071</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name="TextBox 37">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000026000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11008180" y="3985079"/>
-          <a:ext cx="1401534" cy="1770742"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="12700" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="12700" dir="5400000" algn="t" rotWithShape="0">
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="40000"/>
-            </a:schemeClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="900">
-            <a:latin typeface="Century Gothic" charset="0"/>
-            <a:ea typeface="Century Gothic" charset="0"/>
-            <a:cs typeface="Century Gothic" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>4.1.1 Strategically</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t> start social media advertising</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="900" baseline="0">
-            <a:latin typeface="Century Gothic" charset="0"/>
-            <a:ea typeface="Century Gothic" charset="0"/>
-            <a:cs typeface="Century Gothic" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>4.1.2 Send invites</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="900" baseline="0">
-            <a:latin typeface="Century Gothic" charset="0"/>
-            <a:ea typeface="Century Gothic" charset="0"/>
-            <a:cs typeface="Century Gothic" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>4.1.3 Inite people to like page and analyze for comments/feedback</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="900">
-            <a:latin typeface="Century Gothic" charset="0"/>
-            <a:ea typeface="Century Gothic" charset="0"/>
-            <a:cs typeface="Century Gothic" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1898650</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>911678</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>68036</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="TextBox 38">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12403364" y="3985079"/>
-          <a:ext cx="1067707" cy="2165350"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="12700" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="12700" dir="5400000" algn="t" rotWithShape="0">
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="40000"/>
-            </a:schemeClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>4.2.1 Go out on in</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t> the community and talk.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="900" baseline="0">
-            <a:latin typeface="Century Gothic" charset="0"/>
-            <a:ea typeface="Century Gothic" charset="0"/>
-            <a:cs typeface="Century Gothic" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>4.2.2 Do a presentation different places.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="900" baseline="0">
-            <a:latin typeface="Century Gothic" charset="0"/>
-            <a:ea typeface="Century Gothic" charset="0"/>
-            <a:cs typeface="Century Gothic" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>4.2.3 Set up table at local fairs</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="900">
-            <a:latin typeface="Century Gothic" charset="0"/>
-            <a:ea typeface="Century Gothic" charset="0"/>
-            <a:cs typeface="Century Gothic" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1076779</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>204107</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="TextBox 39">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000028000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13636172" y="3985079"/>
-          <a:ext cx="1413328" cy="1811564"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="12700" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="12700" dir="5400000" algn="t" rotWithShape="0">
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-              <a:alpha val="40000"/>
-            </a:schemeClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>4.3.1 Go out and put up Posters at schools &amp; other buildings &amp; walls.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="900" baseline="0">
-            <a:latin typeface="Century Gothic" charset="0"/>
-            <a:ea typeface="Century Gothic" charset="0"/>
-            <a:cs typeface="Century Gothic" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>4.3.2 Hand out flyers around the community and brochures</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="900" baseline="0">
-            <a:latin typeface="Century Gothic" charset="0"/>
-            <a:ea typeface="Century Gothic" charset="0"/>
-            <a:cs typeface="Century Gothic" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Century Gothic" charset="0"/>
-              <a:ea typeface="Century Gothic" charset="0"/>
-              <a:cs typeface="Century Gothic" charset="0"/>
-            </a:rPr>
-            <a:t>4.3.3 Hand out water bottles to students</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5840,7 +4587,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000028000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000028000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6124,33 +4871,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H39"/>
+  <dimension ref="B1:I39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="2" customWidth="1"/>
     <col min="2" max="8" width="27" style="2" customWidth="1"/>
-    <col min="9" max="9" width="3" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.875" style="2" customWidth="1"/>
     <col min="10" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6161,53 +4908,56 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="2:8" ht="13.35" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" ht="13.35" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="16"/>
+      <c r="H3" s="17"/>
     </row>
-    <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="18">
         <v>43304</v>
       </c>
-      <c r="H4" s="16"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="33">
+        <v>43361</v>
+      </c>
     </row>
-    <row r="5" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6224,43 +4974,38 @@
     <row r="30" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="31" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="32" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="21" t="s">
+    <row r="33" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
     </row>
-    <row r="34" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
+    <row r="34" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
     </row>
-    <row r="35" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="14"/>
     </row>
-    <row r="38" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="B33:H34"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B33:H34" r:id="rId1" display="CLICK HERE TO CREATE WBS OUTLINE &amp; DIAGRAM TEMPLATES IN SMARTSHEET"/>
+    <hyperlink ref="B33:H34" r:id="rId1" display="CLICK HERE TO CREATE WBS OUTLINE &amp; DIAGRAM TEMPLATES IN SMARTSHEET" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="59" orientation="landscape" r:id="rId2"/>
@@ -6269,7 +5014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6321,12 +5066,12 @@
     </row>
     <row r="5" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
@@ -6342,141 +5087,141 @@
       <c r="B8" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
     </row>
     <row r="11" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8">
         <v>1.2</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
     </row>
     <row r="13" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
     </row>
     <row r="14" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="8">
         <v>1.3</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
     </row>
     <row r="16" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="8">
         <v>1.4</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
     </row>
     <row r="18" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
     </row>
     <row r="19" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
     </row>
     <row r="20" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="24"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
     </row>
     <row r="22" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7">
@@ -6492,91 +5237,91 @@
       <c r="B23" s="8">
         <v>2.1</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
     </row>
     <row r="24" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="24"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="27"/>
     </row>
     <row r="25" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="24"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
     </row>
     <row r="26" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="28"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
     </row>
     <row r="27" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="24"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="27"/>
     </row>
     <row r="28" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="27"/>
     </row>
     <row r="29" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="8">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="28"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
     </row>
     <row r="30" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="8">
         <v>2.4</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="28"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="24"/>
     </row>
     <row r="31" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="24"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="27"/>
     </row>
     <row r="32" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7">
@@ -6592,108 +5337,136 @@
       <c r="B33" s="8">
         <v>3.1</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="27"/>
-      <c r="E33" s="28"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24"/>
     </row>
     <row r="34" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="24"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="27"/>
     </row>
     <row r="35" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="8">
         <v>3.2</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="24"/>
     </row>
     <row r="36" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="24"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="27"/>
     </row>
     <row r="37" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="8">
         <v>3.3</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="27"/>
-      <c r="E37" s="28"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="24"/>
     </row>
     <row r="38" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="24"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="27"/>
     </row>
     <row r="39" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="8">
         <v>3.4</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="28"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
     </row>
     <row r="40" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="23"/>
-      <c r="E40" s="24"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="27"/>
     </row>
     <row r="41" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D41" s="23"/>
-      <c r="E41" s="24"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="27"/>
     </row>
     <row r="43" spans="2:5" ht="22.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
     </row>
     <row r="44" spans="2:5" ht="22.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="B43:E44"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C14:E14"/>
@@ -6703,37 +5476,9 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="B43:E44"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B43:E44" r:id="rId1" display="CLICK HERE TO CREATE WBS OUTLINE AND DIAGRAM TEMPLATES IN SMARTSHEET"/>
+    <hyperlink ref="B43:E44" r:id="rId1" display="CLICK HERE TO CREATE WBS OUTLINE AND DIAGRAM TEMPLATES IN SMARTSHEET" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>